<commit_message>
updates for inital board design (optics_brd_r001)
</commit_message>
<xml_diff>
--- a/doc/design/comparison_matrix_qp.xlsx
+++ b/doc/design/comparison_matrix_qp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Dropbox\Documents\MS\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Dropbox\Documents\MS\doc\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,56 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v3.0" hidden="1">Sheet1!$A$10</definedName>
-    <definedName name="_xlchart.v3.1" hidden="1">Sheet1!$A$11</definedName>
-    <definedName name="_xlchart.v3.10" hidden="1">Sheet1!$A$9</definedName>
-    <definedName name="_xlchart.v3.11" hidden="1">Sheet1!$H$10:$N$10</definedName>
-    <definedName name="_xlchart.v3.12" hidden="1">Sheet1!$H$11:$N$11</definedName>
-    <definedName name="_xlchart.v3.13" hidden="1">Sheet1!$H$12:$N$12</definedName>
-    <definedName name="_xlchart.v3.14" hidden="1">Sheet1!$H$13:$N$13</definedName>
-    <definedName name="_xlchart.v3.15" hidden="1">Sheet1!$H$2:$N$2</definedName>
-    <definedName name="_xlchart.v3.16" hidden="1">Sheet1!$H$3:$N$3</definedName>
-    <definedName name="_xlchart.v3.17" hidden="1">Sheet1!$H$4:$N$4</definedName>
-    <definedName name="_xlchart.v3.18" hidden="1">Sheet1!$H$5:$N$5</definedName>
-    <definedName name="_xlchart.v3.19" hidden="1">Sheet1!$H$6:$N$6</definedName>
-    <definedName name="_xlchart.v3.2" hidden="1">Sheet1!$A$12</definedName>
-    <definedName name="_xlchart.v3.20" hidden="1">Sheet1!$H$7:$N$7</definedName>
-    <definedName name="_xlchart.v3.21" hidden="1">Sheet1!$H$8:$N$8</definedName>
-    <definedName name="_xlchart.v3.22" hidden="1">Sheet1!$H$9:$N$9</definedName>
-    <definedName name="_xlchart.v3.23" hidden="1">Sheet1!$H$9:$N$9</definedName>
-    <definedName name="_xlchart.v3.24" hidden="1">Sheet1!$A$10</definedName>
-    <definedName name="_xlchart.v3.25" hidden="1">Sheet1!$A$11</definedName>
-    <definedName name="_xlchart.v3.26" hidden="1">Sheet1!$A$12</definedName>
-    <definedName name="_xlchart.v3.27" hidden="1">Sheet1!$A$13</definedName>
-    <definedName name="_xlchart.v3.28" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v3.29" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v3.3" hidden="1">Sheet1!$A$13</definedName>
-    <definedName name="_xlchart.v3.30" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v3.31" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v3.32" hidden="1">Sheet1!$A$7</definedName>
-    <definedName name="_xlchart.v3.33" hidden="1">Sheet1!$A$8</definedName>
-    <definedName name="_xlchart.v3.34" hidden="1">Sheet1!$A$9</definedName>
-    <definedName name="_xlchart.v3.35" hidden="1">Sheet1!$H$10:$N$10</definedName>
-    <definedName name="_xlchart.v3.36" hidden="1">Sheet1!$H$11:$N$11</definedName>
-    <definedName name="_xlchart.v3.37" hidden="1">Sheet1!$H$12:$N$12</definedName>
-    <definedName name="_xlchart.v3.38" hidden="1">Sheet1!$H$13:$N$13</definedName>
-    <definedName name="_xlchart.v3.39" hidden="1">Sheet1!$H$2:$N$2</definedName>
-    <definedName name="_xlchart.v3.4" hidden="1">Sheet1!$A$3</definedName>
-    <definedName name="_xlchart.v3.40" hidden="1">Sheet1!$H$3:$N$3</definedName>
-    <definedName name="_xlchart.v3.41" hidden="1">Sheet1!$H$4:$N$4</definedName>
-    <definedName name="_xlchart.v3.42" hidden="1">Sheet1!$H$5:$N$5</definedName>
-    <definedName name="_xlchart.v3.43" hidden="1">Sheet1!$H$6:$N$6</definedName>
-    <definedName name="_xlchart.v3.44" hidden="1">Sheet1!$H$7:$N$7</definedName>
-    <definedName name="_xlchart.v3.45" hidden="1">Sheet1!$H$8:$N$8</definedName>
-    <definedName name="_xlchart.v3.46" hidden="1">Sheet1!$H$9:$N$9</definedName>
-    <definedName name="_xlchart.v3.47" hidden="1">Sheet1!$H$9:$N$9</definedName>
-    <definedName name="_xlchart.v3.5" hidden="1">Sheet1!$A$4</definedName>
-    <definedName name="_xlchart.v3.6" hidden="1">Sheet1!$A$5</definedName>
-    <definedName name="_xlchart.v3.7" hidden="1">Sheet1!$A$6</definedName>
-    <definedName name="_xlchart.v3.8" hidden="1">Sheet1!$A$7</definedName>
-    <definedName name="_xlchart.v3.9" hidden="1">Sheet1!$A$8</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -671,9 +621,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -731,6 +678,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3446,7 +3396,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V17" sqref="V17"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3456,7 +3406,7 @@
     <col min="3" max="3" width="14.765625" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.3828125" style="5" customWidth="1"/>
     <col min="5" max="5" width="9.53515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.69140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.765625" style="5" customWidth="1"/>
     <col min="7" max="7" width="17.3828125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="14" width="5.921875" style="5" customWidth="1"/>
     <col min="15" max="15" width="17.765625" style="1" customWidth="1"/>
@@ -3471,15 +3421,15 @@
       <c r="E1" s="8"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
       <c r="O1" s="9"/>
       <c r="P1" s="10"/>
     </row>
@@ -3505,31 +3455,31 @@
       <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="27">
         <v>400</v>
       </c>
-      <c r="I2" s="29">
+      <c r="I2" s="28">
         <v>450</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="29">
         <v>480</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="30">
         <v>500</v>
       </c>
-      <c r="L2" s="32">
+      <c r="L2" s="31">
         <v>580</v>
       </c>
-      <c r="M2" s="33">
+      <c r="M2" s="32">
         <v>600</v>
       </c>
-      <c r="N2" s="34">
+      <c r="N2" s="33">
         <v>640</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="36" t="s">
+      <c r="P2" s="35" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3555,29 +3505,29 @@
       <c r="G3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="36">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I3" s="38">
+      <c r="I3" s="37">
         <v>0.19</v>
       </c>
-      <c r="J3" s="39">
+      <c r="J3" s="38">
         <v>0.21</v>
       </c>
-      <c r="K3" s="40">
+      <c r="K3" s="39">
         <v>0.22</v>
       </c>
-      <c r="L3" s="41">
+      <c r="L3" s="40">
         <v>0.31</v>
       </c>
-      <c r="M3" s="42">
+      <c r="M3" s="41">
         <v>0.34499999999999997</v>
       </c>
-      <c r="N3" s="43">
+      <c r="N3" s="42">
         <v>0.4</v>
       </c>
       <c r="O3" s="14"/>
-      <c r="P3" s="44" t="s">
+      <c r="P3" s="43" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3625,7 +3575,7 @@
         <v>0.4</v>
       </c>
       <c r="O4" s="18"/>
-      <c r="P4" s="45" t="s">
+      <c r="P4" s="44" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3673,7 +3623,7 @@
         <v>0.4</v>
       </c>
       <c r="O5" s="22"/>
-      <c r="P5" s="46" t="s">
+      <c r="P5" s="45" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3721,7 +3671,7 @@
         <v>0.4</v>
       </c>
       <c r="O6" s="18"/>
-      <c r="P6" s="45" t="s">
+      <c r="P6" s="44" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3771,7 +3721,7 @@
       <c r="O7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="46" t="s">
+      <c r="P7" s="45" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3819,7 +3769,7 @@
         <v>0.45</v>
       </c>
       <c r="O8" s="18"/>
-      <c r="P8" s="45" t="s">
+      <c r="P8" s="44" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3867,7 +3817,7 @@
         <v>0.42</v>
       </c>
       <c r="O9" s="22"/>
-      <c r="P9" s="46" t="s">
+      <c r="P9" s="45" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3915,7 +3865,7 @@
         <v>0.45</v>
       </c>
       <c r="O10" s="18"/>
-      <c r="P10" s="45" t="s">
+      <c r="P10" s="44" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3963,7 +3913,7 @@
         <v>0.42</v>
       </c>
       <c r="O11" s="22"/>
-      <c r="P11" s="46" t="s">
+      <c r="P11" s="45" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4011,57 +3961,57 @@
         <v>0.42</v>
       </c>
       <c r="O12" s="18"/>
-      <c r="P12" s="45" t="s">
+      <c r="P12" s="44" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="48">
+      <c r="B13" s="47">
         <v>156.44</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="49">
+      <c r="D13" s="48">
         <v>633</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="E13" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="49">
+      <c r="F13" s="48">
         <v>24.35</v>
       </c>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="49">
+      <c r="H13" s="48">
         <v>0.09</v>
       </c>
-      <c r="I13" s="49">
+      <c r="I13" s="48">
         <v>0.18</v>
       </c>
-      <c r="J13" s="49">
+      <c r="J13" s="48">
         <v>0.20499999999999999</v>
       </c>
-      <c r="K13" s="49">
+      <c r="K13" s="48">
         <v>0.22500000000000001</v>
       </c>
-      <c r="L13" s="49">
+      <c r="L13" s="48">
         <v>0.35</v>
       </c>
-      <c r="M13" s="49">
+      <c r="M13" s="48">
         <v>0.38</v>
       </c>
-      <c r="N13" s="49">
+      <c r="N13" s="48">
         <v>0.42</v>
       </c>
-      <c r="O13" s="47" t="s">
+      <c r="O13" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="P13" s="27" t="s">
+      <c r="P13" s="26" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>